<commit_message>
WorkflowAnalysisValidatorCounter and workflowAnalysisConditionsCounter add
</commit_message>
<xml_diff>
--- a/Data Files/ComponentVersionScheme.xlsx
+++ b/Data Files/ComponentVersionScheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="22995" windowHeight="10050" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="22995" windowHeight="10050" tabRatio="500" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="WorkflowType" sheetId="5" r:id="rId5"/>
     <sheet name="WorkflowScreen" sheetId="6" r:id="rId6"/>
     <sheet name="PostFunctionCounter" sheetId="7" r:id="rId7"/>
+    <sheet name="ConditionsCounter" sheetId="8" r:id="rId8"/>
+    <sheet name="ValidatorsCounter" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>clickableTab</t>
   </si>
@@ -252,6 +254,18 @@
   </si>
   <si>
     <t>//span[contains(., 'BarfedBackFood')]/ancestor::tr/td[contains(., 'Custom')]/aui-badge[@class='aui-badge-primary']</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Eating')]/ancestor::tr/td[5]/aui-badge</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Create')]/ancestor::tr/td[6]/aui-badge</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Create')]/ancestor::tr/td[5]</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Eating')]/ancestor::tr/td[6]</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,4 +1208,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New features test is done
</commit_message>
<xml_diff>
--- a/Data Files/ComponentVersionScheme.xlsx
+++ b/Data Files/ComponentVersionScheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="22995" windowHeight="10050" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="22995" windowHeight="10050" tabRatio="500" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="PostFunctionCounter" sheetId="7" r:id="rId7"/>
     <sheet name="ConditionsCounter" sheetId="8" r:id="rId8"/>
     <sheet name="ValidatorsCounter" sheetId="9" r:id="rId9"/>
+    <sheet name="PostFunctionText" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>clickableTab</t>
   </si>
@@ -266,6 +267,30 @@
   </si>
   <si>
     <t>//span[contains(., 'Eating')]/ancestor::tr/td[6]</t>
+  </si>
+  <si>
+    <t>rowXpath</t>
+  </si>
+  <si>
+    <t>postFunctionsList</t>
+  </si>
+  <si>
+    <t>//tr[@class='transition-details-row']/td/div/div[@id='glass-transitions-postfunctions-panel-1']/div/div/ol/li</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Create')]/ancestor::td[@class='transition-name']</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'Eating')]/ancestor::td[@class='transition-name']</t>
+  </si>
+  <si>
+    <t>//span[contains(., 'BarfedBackFood')]/ancestor::td[@class='transition-name']</t>
+  </si>
+  <si>
+    <t>//tr[@class='transition-details-row']/td/div/div[@id='glass-transitions-postfunctions-panel-2']/div/div/ol/li</t>
+  </si>
+  <si>
+    <t>//tr[@class='transition-details-row']/td/div/div[@id='glass-transitions-postfunctions-panel-4']/div/div/ol/li</t>
   </si>
 </sst>
 </file>
@@ -833,6 +858,70 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="97" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
@@ -1156,7 +1245,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1304,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>